<commit_message>
fix the test data file
</commit_message>
<xml_diff>
--- a/src/app/app-playloader/data/sample.05.xlsx
+++ b/src/app/app-playloader/data/sample.05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/src/app/app-playloader/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F95F47F-66DD-B54E-9259-CF6C3ECF3008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE90B7F-A08A-514C-ABCA-1A7D04306E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>funds.2.investmentAmt</t>
-  </si>
-  <si>
-    <t>list.ob.num</t>
   </si>
   <si>
     <t>funds.2.investmentcury</t>
@@ -544,7 +541,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C19" sqref="C19:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -655,16 +652,16 @@
     </row>
     <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -672,7 +669,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -763,7 +760,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd hh:mm:ss.000Z")</f>
-        <v>2024-04-04 17:19:43.210Z</v>
+        <v>2024-04-04 17:28:34.590Z</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -796,10 +793,10 @@
     </row>
     <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>31</v>
@@ -815,7 +812,7 @@
       <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -830,7 +827,7 @@
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D20" s="2">
         <v>1000</v>
@@ -838,24 +835,24 @@
     </row>
     <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
fix the "false"  boolean value case
</commit_message>
<xml_diff>
--- a/src/app/app-playloader/data/sample.05.xlsx
+++ b/src/app/app-playloader/data/sample.05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/src/app/app-playloader/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63683C70-4162-D244-9E41-E2A715AC03BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781695D0-D422-BC43-AAE9-99291971D6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,58 +118,58 @@
     <t>isCertified</t>
   </si>
   <si>
+    <t>intructionDateTime</t>
+  </si>
+  <si>
+    <t>funds.1.code</t>
+  </si>
+  <si>
+    <t>list.obj.str</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>funds.1.investmentAmt</t>
+  </si>
+  <si>
+    <t>list.obj.num</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>funds.2.code</t>
+  </si>
+  <si>
+    <t>EFGH</t>
+  </si>
+  <si>
+    <t>funds.2.investmentAmt</t>
+  </si>
+  <si>
+    <t>funds.2.investmentcury</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>funds.1.investmentcury</t>
+  </si>
+  <si>
+    <t>category.2</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>totalamount</t>
+  </si>
+  <si>
+    <t>isSigned</t>
+  </si>
+  <si>
     <t>boolean</t>
-  </si>
-  <si>
-    <t>intructionDateTime</t>
-  </si>
-  <si>
-    <t>funds.1.code</t>
-  </si>
-  <si>
-    <t>list.obj.str</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>funds.1.investmentAmt</t>
-  </si>
-  <si>
-    <t>list.obj.num</t>
-  </si>
-  <si>
-    <t>HKD</t>
-  </si>
-  <si>
-    <t>funds.2.code</t>
-  </si>
-  <si>
-    <t>EFGH</t>
-  </si>
-  <si>
-    <t>funds.2.investmentAmt</t>
-  </si>
-  <si>
-    <t>funds.2.investmentcury</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>funds.1.investmentcury</t>
-  </si>
-  <si>
-    <t>category.2</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>totalamount</t>
-  </si>
-  <si>
-    <t>isSigned</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -652,16 +652,16 @@
     </row>
     <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -669,7 +669,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -741,124 +741,124 @@
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="C14" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f ca="1">TEXT(NOW(), "yyyy-mm-dd hh:mm:ss.000Z")</f>
-        <v>2024-04-04 17:45:54.660Z</v>
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f ca="1">TEXT(NOW(), "yyyy-mm-dd hh:mm:ss.000Z")</f>
+        <v>2024-04-04 22:46:47.290Z</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>20000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="1" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="1" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>